<commit_message>
fix revenue and user data
</commit_message>
<xml_diff>
--- a/user-data/uganda-life-expectancy/uganda-life-expectancy.xlsx
+++ b/user-data/uganda-life-expectancy/uganda-life-expectancy.xlsx
@@ -1389,7 +1389,7 @@
         <v>2014</v>
       </c>
       <c r="D16" t="n">
-        <v>48.9</v>
+        <v>41</v>
       </c>
     </row>
     <row r="17">
@@ -2927,7 +2927,7 @@
         <v>33</v>
       </c>
       <c r="C16" t="n">
-        <v>48.9</v>
+        <v>41</v>
       </c>
     </row>
     <row r="17">

</xml_diff>